<commit_message>
revised based on Meng's comments
</commit_message>
<xml_diff>
--- a/slides/report/newStar/images/funding.xlsx
+++ b/slides/report/newStar/images/funding.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\MEGAsync\Nutstore\Presentation_slides\slides\report\newStar\images\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{CF5355FF-B8CC-4EFB-86A4-E282DA1BD2B3}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{6980147B-F3F9-463F-915B-64890EE7F3E4}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="57840" windowHeight="15720" xr2:uid="{9CCFCCB2-6DA2-4FFF-B873-420485C0C63A}"/>
   </bookViews>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="83" uniqueCount="73">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="83" uniqueCount="70">
   <si>
     <t>序号</t>
   </si>
@@ -74,20 +74,6 @@
     <t>20/20</t>
   </si>
   <si>
-    <r>
-      <t>负责人</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="10"/>
-        <color theme="1"/>
-        <rFont val="Times New Roman"/>
-        <family val="1"/>
-      </rPr>
-      <t xml:space="preserve">1 </t>
-    </r>
-  </si>
-  <si>
     <t>突发公共卫生事件互联网政治生态与话语竞争研究</t>
   </si>
   <si>
@@ -97,20 +83,6 @@
     <t>2020-12~2023-06</t>
   </si>
   <si>
-    <r>
-      <t>负责人</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="10"/>
-        <color theme="1"/>
-        <rFont val="Times New Roman"/>
-        <family val="1"/>
-      </rPr>
-      <t>1</t>
-    </r>
-  </si>
-  <si>
     <t>新型城镇化进程中身份认同危机与语言治理</t>
   </si>
   <si>
@@ -118,20 +90,6 @@
   </si>
   <si>
     <t>2020-09~2021-08</t>
-  </si>
-  <si>
-    <r>
-      <t>负责人</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="10"/>
-        <color theme="1"/>
-        <rFont val="Times New Roman"/>
-        <family val="1"/>
-      </rPr>
-      <t xml:space="preserve"> 1</t>
-    </r>
   </si>
   <si>
     <t>北京市违法建设专题研究</t>
@@ -218,9 +176,6 @@
   </si>
   <si>
     <t>春风基金</t>
-  </si>
-  <si>
-    <t>负责人1</t>
   </si>
   <si>
     <t>6/6</t>
@@ -318,6 +273,9 @@
   </si>
   <si>
     <t>国家高端智库</t>
+  </si>
+  <si>
+    <t>负责人</t>
   </si>
 </sst>
 </file>
@@ -812,7 +770,7 @@
   <dimension ref="A1:F13"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C8" sqref="C8"/>
+      <selection activeCell="H7" sqref="H7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -831,7 +789,7 @@
         <v>3</v>
       </c>
       <c r="E1" s="2" t="s">
-        <v>50</v>
+        <v>46</v>
       </c>
       <c r="F1" s="2" t="s">
         <v>4</v>
@@ -854,7 +812,7 @@
         <v>8</v>
       </c>
       <c r="F2" s="8" t="s">
-        <v>46</v>
+        <v>69</v>
       </c>
     </row>
     <row r="3" spans="1:6" ht="60.75" thickBot="1" x14ac:dyDescent="0.3">
@@ -865,7 +823,7 @@
         <v>9</v>
       </c>
       <c r="C3" s="5" t="s">
-        <v>71</v>
+        <v>67</v>
       </c>
       <c r="D3" s="6" t="s">
         <v>10</v>
@@ -874,7 +832,7 @@
         <v>11</v>
       </c>
       <c r="F3" s="5" t="s">
-        <v>12</v>
+        <v>69</v>
       </c>
     </row>
     <row r="4" spans="1:6" ht="72.75" thickBot="1" x14ac:dyDescent="0.3">
@@ -882,19 +840,19 @@
         <v>3</v>
       </c>
       <c r="B4" s="4" t="s">
+        <v>12</v>
+      </c>
+      <c r="C4" s="5" t="s">
         <v>13</v>
       </c>
-      <c r="C4" s="5" t="s">
+      <c r="D4" s="6" t="s">
         <v>14</v>
       </c>
-      <c r="D4" s="6" t="s">
-        <v>15</v>
-      </c>
       <c r="E4" s="16" t="s">
-        <v>47</v>
+        <v>43</v>
       </c>
       <c r="F4" s="5" t="s">
-        <v>16</v>
+        <v>69</v>
       </c>
     </row>
     <row r="5" spans="1:6" ht="60.75" thickBot="1" x14ac:dyDescent="0.3">
@@ -902,19 +860,19 @@
         <v>4</v>
       </c>
       <c r="B5" s="4" t="s">
+        <v>15</v>
+      </c>
+      <c r="C5" s="5" t="s">
+        <v>16</v>
+      </c>
+      <c r="D5" s="6" t="s">
         <v>17</v>
       </c>
-      <c r="C5" s="5" t="s">
-        <v>18</v>
-      </c>
-      <c r="D5" s="6" t="s">
-        <v>19</v>
-      </c>
       <c r="E5" s="16" t="s">
-        <v>48</v>
+        <v>44</v>
       </c>
       <c r="F5" s="7" t="s">
-        <v>20</v>
+        <v>69</v>
       </c>
     </row>
     <row r="6" spans="1:6" ht="41.25" thickBot="1" x14ac:dyDescent="0.3">
@@ -922,19 +880,19 @@
         <v>5</v>
       </c>
       <c r="B6" s="4" t="s">
+        <v>18</v>
+      </c>
+      <c r="C6" s="5" t="s">
+        <v>19</v>
+      </c>
+      <c r="D6" s="6" t="s">
+        <v>20</v>
+      </c>
+      <c r="E6" s="14" t="s">
         <v>21</v>
       </c>
-      <c r="C6" s="5" t="s">
-        <v>22</v>
-      </c>
-      <c r="D6" s="6" t="s">
-        <v>23</v>
-      </c>
-      <c r="E6" s="14" t="s">
-        <v>24</v>
-      </c>
       <c r="F6" s="7" t="s">
-        <v>16</v>
+        <v>69</v>
       </c>
     </row>
     <row r="7" spans="1:6" ht="48.75" thickBot="1" x14ac:dyDescent="0.3">
@@ -942,19 +900,19 @@
         <v>6</v>
       </c>
       <c r="B7" s="4" t="s">
-        <v>25</v>
+        <v>22</v>
       </c>
       <c r="C7" s="5" t="s">
-        <v>26</v>
+        <v>23</v>
       </c>
       <c r="D7" s="6" t="s">
-        <v>27</v>
+        <v>24</v>
       </c>
       <c r="E7" s="16" t="s">
-        <v>49</v>
+        <v>45</v>
       </c>
       <c r="F7" s="7" t="s">
-        <v>16</v>
+        <v>69</v>
       </c>
     </row>
     <row r="8" spans="1:6" ht="60.75" thickBot="1" x14ac:dyDescent="0.3">
@@ -962,19 +920,19 @@
         <v>7</v>
       </c>
       <c r="B8" s="4" t="s">
+        <v>64</v>
+      </c>
+      <c r="C8" s="5" t="s">
         <v>68</v>
       </c>
-      <c r="C8" s="5" t="s">
-        <v>72</v>
-      </c>
       <c r="D8" s="6" t="s">
-        <v>69</v>
+        <v>65</v>
       </c>
       <c r="E8" s="16" t="s">
-        <v>70</v>
+        <v>66</v>
       </c>
       <c r="F8" s="7" t="s">
-        <v>51</v>
+        <v>47</v>
       </c>
     </row>
     <row r="9" spans="1:6" ht="60.75" thickBot="1" x14ac:dyDescent="0.3">
@@ -982,19 +940,19 @@
         <v>8</v>
       </c>
       <c r="B9" s="4" t="s">
+        <v>25</v>
+      </c>
+      <c r="C9" s="5" t="s">
+        <v>26</v>
+      </c>
+      <c r="D9" s="6" t="s">
+        <v>27</v>
+      </c>
+      <c r="E9" s="14" t="s">
         <v>28</v>
       </c>
-      <c r="C9" s="5" t="s">
-        <v>29</v>
-      </c>
-      <c r="D9" s="6" t="s">
-        <v>30</v>
-      </c>
-      <c r="E9" s="14" t="s">
-        <v>31</v>
-      </c>
       <c r="F9" s="7" t="s">
-        <v>51</v>
+        <v>47</v>
       </c>
     </row>
     <row r="10" spans="1:6" ht="60.75" thickBot="1" x14ac:dyDescent="0.3">
@@ -1002,19 +960,19 @@
         <v>9</v>
       </c>
       <c r="B10" s="4" t="s">
+        <v>29</v>
+      </c>
+      <c r="C10" s="5" t="s">
+        <v>30</v>
+      </c>
+      <c r="D10" s="6" t="s">
+        <v>31</v>
+      </c>
+      <c r="E10" s="14" t="s">
         <v>32</v>
       </c>
-      <c r="C10" s="5" t="s">
-        <v>33</v>
-      </c>
-      <c r="D10" s="6" t="s">
-        <v>34</v>
-      </c>
-      <c r="E10" s="14" t="s">
-        <v>35</v>
-      </c>
       <c r="F10" s="7" t="s">
-        <v>51</v>
+        <v>47</v>
       </c>
     </row>
     <row r="11" spans="1:6" ht="48.75" thickBot="1" x14ac:dyDescent="0.3">
@@ -1022,19 +980,19 @@
         <v>10</v>
       </c>
       <c r="B11" s="4" t="s">
-        <v>36</v>
+        <v>33</v>
       </c>
       <c r="C11" s="5" t="s">
-        <v>45</v>
+        <v>42</v>
       </c>
       <c r="D11" s="6" t="s">
-        <v>19</v>
+        <v>17</v>
       </c>
       <c r="E11" s="14" t="s">
-        <v>37</v>
+        <v>34</v>
       </c>
       <c r="F11" s="7" t="s">
-        <v>51</v>
+        <v>47</v>
       </c>
     </row>
     <row r="12" spans="1:6" ht="72.75" thickBot="1" x14ac:dyDescent="0.3">
@@ -1042,19 +1000,19 @@
         <v>11</v>
       </c>
       <c r="B12" s="4" t="s">
-        <v>38</v>
+        <v>35</v>
       </c>
       <c r="C12" s="5" t="s">
-        <v>33</v>
+        <v>30</v>
       </c>
       <c r="D12" s="6" t="s">
-        <v>39</v>
+        <v>36</v>
       </c>
       <c r="E12" s="15" t="s">
-        <v>40</v>
+        <v>37</v>
       </c>
       <c r="F12" s="7" t="s">
-        <v>51</v>
+        <v>47</v>
       </c>
     </row>
     <row r="13" spans="1:6" ht="72.75" thickBot="1" x14ac:dyDescent="0.3">
@@ -1062,19 +1020,19 @@
         <v>12</v>
       </c>
       <c r="B13" s="5" t="s">
+        <v>38</v>
+      </c>
+      <c r="C13" s="5" t="s">
+        <v>39</v>
+      </c>
+      <c r="D13" s="6" t="s">
+        <v>40</v>
+      </c>
+      <c r="E13" s="14" t="s">
         <v>41</v>
       </c>
-      <c r="C13" s="5" t="s">
-        <v>42</v>
-      </c>
-      <c r="D13" s="6" t="s">
-        <v>43</v>
-      </c>
-      <c r="E13" s="14" t="s">
-        <v>44</v>
-      </c>
       <c r="F13" s="7" t="s">
-        <v>51</v>
+        <v>47</v>
       </c>
     </row>
   </sheetData>
@@ -1095,70 +1053,70 @@
   <sheetData>
     <row r="1" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
-        <v>52</v>
+        <v>48</v>
       </c>
       <c r="B1" t="s">
-        <v>53</v>
+        <v>49</v>
       </c>
       <c r="C1" t="s">
-        <v>54</v>
+        <v>50</v>
       </c>
       <c r="D1" t="s">
-        <v>55</v>
+        <v>51</v>
       </c>
       <c r="E1" t="s">
-        <v>62</v>
+        <v>58</v>
       </c>
     </row>
     <row r="2" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
-        <v>56</v>
+        <v>52</v>
       </c>
       <c r="B2">
         <v>2022</v>
       </c>
       <c r="C2" t="s">
-        <v>57</v>
+        <v>53</v>
       </c>
       <c r="D2" t="s">
-        <v>58</v>
+        <v>54</v>
       </c>
       <c r="E2" t="s">
-        <v>63</v>
+        <v>59</v>
       </c>
     </row>
     <row r="3" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
-        <v>59</v>
+        <v>55</v>
       </c>
       <c r="B3">
         <v>2020</v>
       </c>
       <c r="C3" t="s">
-        <v>60</v>
+        <v>56</v>
       </c>
       <c r="D3" t="s">
-        <v>61</v>
+        <v>57</v>
       </c>
       <c r="E3" t="s">
-        <v>67</v>
+        <v>63</v>
       </c>
     </row>
     <row r="4" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
-        <v>59</v>
+        <v>55</v>
       </c>
       <c r="B4">
         <v>2020</v>
       </c>
       <c r="C4" t="s">
-        <v>64</v>
+        <v>60</v>
       </c>
       <c r="D4" t="s">
-        <v>65</v>
+        <v>61</v>
       </c>
       <c r="E4" t="s">
-        <v>66</v>
+        <v>62</v>
       </c>
     </row>
   </sheetData>

</xml_diff>